<commit_message>
work done on results, intro and method sections of report
</commit_message>
<xml_diff>
--- a/ADS Coursework - TSP/report/experimental_data.xlsx
+++ b/ADS Coursework - TSP/report/experimental_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Work\ADS\cw repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Work\ADS\cw repo\ADS Coursework - TSP\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -232,23 +232,29 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5949,7 +5955,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5960,7 +5966,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5971,7 +5977,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="105" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -5983,7 +5989,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="105" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -5995,7 +6001,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="105" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -6007,7 +6013,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9310872" cy="6084186"/>
+    <xdr:ext cx="9308171" cy="6078963"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6061,7 +6067,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10261023" cy="7143750"/>
+    <xdr:ext cx="10269682" cy="7143750"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6088,7 +6094,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10261023" cy="7143750"/>
+    <xdr:ext cx="10287000" cy="7157357"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6115,7 +6121,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10261023" cy="7143750"/>
+    <xdr:ext cx="10287000" cy="7157357"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6403,8 +6409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="T35" sqref="T35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6434,64 +6440,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="H1" s="13" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="H1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="N1" s="13" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="N1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="T1" s="13" t="s">
+      <c r="O1" s="16"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="T1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="13"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="H2" s="15" t="s">
+      <c r="E2" s="18"/>
+      <c r="H2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="N2" s="15" t="s">
+      <c r="K2" s="13"/>
+      <c r="N2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="16" t="s">
+      <c r="O2" s="13"/>
+      <c r="P2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="T2" s="15" t="s">
+      <c r="Q2" s="13"/>
+      <c r="T2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="16" t="s">
+      <c r="U2" s="13"/>
+      <c r="V2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="15"/>
+      <c r="W2" s="13"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -7254,64 +7260,64 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="H15" s="13" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="H15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="N15" s="13" t="s">
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="N15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="O15" s="13"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="T15" s="13" t="s">
+      <c r="O15" s="16"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="T15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="U15" s="13"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="H16" s="15" t="s">
+      <c r="E16" s="13"/>
+      <c r="H16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="14"/>
+      <c r="J16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="15"/>
-      <c r="N16" s="15" t="s">
+      <c r="K16" s="13"/>
+      <c r="N16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O16" s="18"/>
-      <c r="P16" s="16" t="s">
+      <c r="O16" s="14"/>
+      <c r="P16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="15"/>
-      <c r="T16" s="15" t="s">
+      <c r="Q16" s="13"/>
+      <c r="T16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="U16" s="18"/>
-      <c r="V16" s="16" t="s">
+      <c r="U16" s="14"/>
+      <c r="V16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="W16" s="15"/>
+      <c r="W16" s="13"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -8015,22 +8021,22 @@
         <f>AVERAGE(E18:E27)</f>
         <v>41982.406971895092</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="22" t="s">
         <v>16</v>
       </c>
       <c r="H28">
         <f>AVERAGE(H18:H27)</f>
         <v>13.3</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="9">
         <f>AVERAGE(I18:I27)</f>
         <v>296543.88905721199</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="12">
         <f>AVERAGE(J18:J27)</f>
         <v>1102.4000000000001</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="9">
         <f>AVERAGE(K18:K27)</f>
         <v>281530.52104881068</v>
       </c>
@@ -8041,7 +8047,7 @@
         <f>AVERAGE(N18:N27)</f>
         <v>44.2</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="9">
         <f>AVERAGE(O18:O27)</f>
         <v>90517.890018195598</v>
       </c>
@@ -8049,7 +8055,7 @@
         <f>AVERAGE(P18:P27)</f>
         <v>8113.1</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="9">
         <f>AVERAGE(Q18:Q27)</f>
         <v>87664.56789116397</v>
       </c>
@@ -8074,37 +8080,37 @@
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="N29" s="13" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="N29" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
       <c r="V29" s="11"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="16" t="s">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="N30" s="15" t="s">
+      <c r="E30" s="13"/>
+      <c r="N30" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O30" s="18"/>
-      <c r="P30" s="16" t="s">
+      <c r="O30" s="14"/>
+      <c r="P30" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q30" s="15"/>
+      <c r="Q30" s="13"/>
       <c r="V30" s="11"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
@@ -8163,7 +8169,7 @@
         <f>AVERAGE(B4:B13)</f>
         <v>0.6</v>
       </c>
-      <c r="O32" s="10">
+      <c r="O32" s="21">
         <f>AVERAGE(C4:C13)</f>
         <v>8980.9182793291875</v>
       </c>
@@ -8199,7 +8205,7 @@
         <f>AVERAGE(H4:H13)</f>
         <v>1</v>
       </c>
-      <c r="O33" s="10">
+      <c r="O33" s="21">
         <f>AVERAGE(I4:I13)</f>
         <v>825.24232272774384</v>
       </c>
@@ -8235,7 +8241,7 @@
         <f>AVERAGE(N4:N13)</f>
         <v>1.6</v>
       </c>
-      <c r="O34" s="10">
+      <c r="O34" s="21">
         <f>AVERAGE(O4:O13)</f>
         <v>54669.0264149633</v>
       </c>
@@ -8271,7 +8277,7 @@
         <f>AVERAGE(T4:T13)</f>
         <v>5.8</v>
       </c>
-      <c r="O35" s="10">
+      <c r="O35" s="21">
         <f>AVERAGE(U4:U13)</f>
         <v>3241.4668367219497</v>
       </c>
@@ -8307,7 +8313,7 @@
         <f>AVERAGE(B18:B27)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="O36" s="10">
+      <c r="O36" s="21">
         <f>AVERAGE(C18:C27)</f>
         <v>43646.373961317106</v>
       </c>
@@ -8343,7 +8349,7 @@
         <f>AVERAGE(H18:H27)</f>
         <v>13.3</v>
       </c>
-      <c r="O37" s="10">
+      <c r="O37" s="21">
         <f>AVERAGE(I18:I27)</f>
         <v>296543.88905721199</v>
       </c>
@@ -8379,7 +8385,7 @@
         <f>AVERAGE(N18:N27)</f>
         <v>44.2</v>
       </c>
-      <c r="O38" s="10">
+      <c r="O38" s="21">
         <f>AVERAGE(O18:O27)</f>
         <v>90517.890018195598</v>
       </c>
@@ -8415,7 +8421,7 @@
         <f>AVERAGE(T18:T27)</f>
         <v>137.1</v>
       </c>
-      <c r="O39" s="10">
+      <c r="O39" s="21">
         <f>AVERAGE(U18:U27)</f>
         <v>35362.50655728639</v>
       </c>
@@ -8451,7 +8457,7 @@
         <f>AVERAGE(B32:B41)</f>
         <v>336.4</v>
       </c>
-      <c r="O40" s="10">
+      <c r="O40" s="21">
         <f>AVERAGE(C32:C41)</f>
         <v>707498.63075170584</v>
       </c>
@@ -8506,22 +8512,22 @@
         <f>AVERAGE(E32:E41)</f>
         <v>672798.02977894177</v>
       </c>
-      <c r="N42" s="13" t="s">
+      <c r="N42" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N43" s="15" t="s">
+      <c r="N43" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O43" s="18"/>
-      <c r="P43" s="16" t="s">
+      <c r="O43" s="14"/>
+      <c r="P43" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q43" s="15"/>
+      <c r="Q43" s="13"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M44" s="7" t="s">
@@ -8548,7 +8554,7 @@
         <f>N32/N32</f>
         <v>1</v>
       </c>
-      <c r="O45" s="12">
+      <c r="O45" s="19">
         <f>O32/O32</f>
         <v>1</v>
       </c>
@@ -8578,7 +8584,7 @@
         <f t="shared" ref="N46:N53" si="0">N33/N33</f>
         <v>1</v>
       </c>
-      <c r="O46" s="12">
+      <c r="O46" s="20">
         <f t="shared" ref="O46:O53" si="1">O33/O33</f>
         <v>1</v>
       </c>
@@ -8608,7 +8614,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O47" s="12">
+      <c r="O47" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8630,7 +8636,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O48" s="12">
+      <c r="O48" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8652,7 +8658,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O49" s="12">
+      <c r="O49" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8674,7 +8680,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O50" s="12">
+      <c r="O50" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8696,7 +8702,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O51" s="12">
+      <c r="O51" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8718,7 +8724,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O52" s="12">
+      <c r="O52" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8740,7 +8746,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O53" s="12">
+      <c r="O53" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8758,23 +8764,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="J16:K16"/>
     <mergeCell ref="N15:Q15"/>
     <mergeCell ref="T15:W15"/>
     <mergeCell ref="B15:E15"/>
@@ -8791,6 +8780,23 @@
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
onto results section of report
</commit_message>
<xml_diff>
--- a/ADS Coursework - TSP/report/experimental_data.xlsx
+++ b/ADS Coursework - TSP/report/experimental_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -232,14 +232,11 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,14 +244,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -307,14 +307,17 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Average</a:t>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Efficacy of Both Algorithms Compared</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Route Length Results Over Multiple Problem Instances of Different Sizes</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
+            <a:endParaRPr lang="en-GB" sz="1800">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -599,14 +602,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1400"/>
                   <a:t>Number</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
                   <a:t> of Cities, n</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB"/>
+                <a:endParaRPr lang="en-GB" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -712,7 +715,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -725,7 +728,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
                   <a:t>Route Length / units</a:t>
                 </a:r>
               </a:p>
@@ -752,7 +755,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -784,7 +787,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -826,7 +829,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -859,12 +862,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -916,15 +914,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" sz="1400" b="0" i="0" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Average Route Length Results as a Ratio</a:t>
+              <a:t>Efficacy of Both Algorithms Compared Using Ratios</a:t>
             </a:r>
-            <a:endParaRPr lang="en-GB" sz="1400">
+            <a:endParaRPr lang="en-GB">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -1162,7 +1157,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1175,7 +1170,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
@@ -1205,7 +1200,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1243,7 +1238,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1308,7 +1303,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
@@ -1370,7 +1365,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1413,7 +1408,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1438,12 +1433,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -5955,10 +5945,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="104" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -5966,10 +5957,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="104" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -6001,7 +5993,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="105" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -6013,7 +6005,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9308171" cy="6078963"/>
+    <xdr:ext cx="10276010" cy="7162067"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6040,7 +6032,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9310872" cy="6084186"/>
+    <xdr:ext cx="10276010" cy="7162067"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6067,7 +6059,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10269682" cy="7143750"/>
+    <xdr:ext cx="10287000" cy="7157357"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6409,8 +6401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43:Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6440,64 +6432,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="H1" s="16" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="H1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="N1" s="16" t="s">
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="N1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="T1" s="16" t="s">
+      <c r="O1" s="17"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="T1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="16"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="H2" s="13" t="s">
+      <c r="E2" s="21"/>
+      <c r="H2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="15" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="N2" s="13" t="s">
+      <c r="K2" s="19"/>
+      <c r="N2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="15" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="T2" s="13" t="s">
+      <c r="Q2" s="19"/>
+      <c r="T2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="13"/>
-      <c r="V2" s="15" t="s">
+      <c r="U2" s="19"/>
+      <c r="V2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="13"/>
+      <c r="W2" s="19"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -7260,64 +7252,64 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="H15" s="16" t="s">
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="H15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="N15" s="16" t="s">
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="N15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="O15" s="16"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="T15" s="16" t="s">
+      <c r="O15" s="17"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="T15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="U15" s="16"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="22"/>
+      <c r="D16" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="H16" s="13" t="s">
+      <c r="E16" s="19"/>
+      <c r="H16" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15" t="s">
+      <c r="I16" s="22"/>
+      <c r="J16" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="13"/>
-      <c r="N16" s="13" t="s">
+      <c r="K16" s="19"/>
+      <c r="N16" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="O16" s="14"/>
-      <c r="P16" s="15" t="s">
+      <c r="O16" s="22"/>
+      <c r="P16" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="13"/>
-      <c r="T16" s="13" t="s">
+      <c r="Q16" s="19"/>
+      <c r="T16" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U16" s="14"/>
-      <c r="V16" s="15" t="s">
+      <c r="U16" s="22"/>
+      <c r="V16" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="W16" s="13"/>
+      <c r="W16" s="19"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -8021,7 +8013,7 @@
         <f>AVERAGE(E18:E27)</f>
         <v>41982.406971895092</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="16" t="s">
         <v>16</v>
       </c>
       <c r="H28">
@@ -8080,37 +8072,37 @@
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="N29" s="16" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="N29" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
       <c r="V29" s="11"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15" t="s">
+      <c r="C30" s="22"/>
+      <c r="D30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="N30" s="13" t="s">
+      <c r="E30" s="19"/>
+      <c r="N30" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="O30" s="14"/>
-      <c r="P30" s="15" t="s">
+      <c r="O30" s="22"/>
+      <c r="P30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="Q30" s="13"/>
+      <c r="Q30" s="19"/>
       <c r="V30" s="11"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
@@ -8169,7 +8161,7 @@
         <f>AVERAGE(B4:B13)</f>
         <v>0.6</v>
       </c>
-      <c r="O32" s="21">
+      <c r="O32" s="15">
         <f>AVERAGE(C4:C13)</f>
         <v>8980.9182793291875</v>
       </c>
@@ -8205,7 +8197,7 @@
         <f>AVERAGE(H4:H13)</f>
         <v>1</v>
       </c>
-      <c r="O33" s="21">
+      <c r="O33" s="15">
         <f>AVERAGE(I4:I13)</f>
         <v>825.24232272774384</v>
       </c>
@@ -8241,7 +8233,7 @@
         <f>AVERAGE(N4:N13)</f>
         <v>1.6</v>
       </c>
-      <c r="O34" s="21">
+      <c r="O34" s="15">
         <f>AVERAGE(O4:O13)</f>
         <v>54669.0264149633</v>
       </c>
@@ -8277,7 +8269,7 @@
         <f>AVERAGE(T4:T13)</f>
         <v>5.8</v>
       </c>
-      <c r="O35" s="21">
+      <c r="O35" s="15">
         <f>AVERAGE(U4:U13)</f>
         <v>3241.4668367219497</v>
       </c>
@@ -8313,7 +8305,7 @@
         <f>AVERAGE(B18:B27)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="O36" s="21">
+      <c r="O36" s="15">
         <f>AVERAGE(C18:C27)</f>
         <v>43646.373961317106</v>
       </c>
@@ -8349,7 +8341,7 @@
         <f>AVERAGE(H18:H27)</f>
         <v>13.3</v>
       </c>
-      <c r="O37" s="21">
+      <c r="O37" s="15">
         <f>AVERAGE(I18:I27)</f>
         <v>296543.88905721199</v>
       </c>
@@ -8385,7 +8377,7 @@
         <f>AVERAGE(N18:N27)</f>
         <v>44.2</v>
       </c>
-      <c r="O38" s="21">
+      <c r="O38" s="15">
         <f>AVERAGE(O18:O27)</f>
         <v>90517.890018195598</v>
       </c>
@@ -8421,7 +8413,7 @@
         <f>AVERAGE(T18:T27)</f>
         <v>137.1</v>
       </c>
-      <c r="O39" s="21">
+      <c r="O39" s="15">
         <f>AVERAGE(U18:U27)</f>
         <v>35362.50655728639</v>
       </c>
@@ -8457,7 +8449,7 @@
         <f>AVERAGE(B32:B41)</f>
         <v>336.4</v>
       </c>
-      <c r="O40" s="21">
+      <c r="O40" s="15">
         <f>AVERAGE(C32:C41)</f>
         <v>707498.63075170584</v>
       </c>
@@ -8512,22 +8504,22 @@
         <f>AVERAGE(E32:E41)</f>
         <v>672798.02977894177</v>
       </c>
-      <c r="N42" s="16" t="s">
+      <c r="N42" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O42" s="16"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="16"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N43" s="13" t="s">
+      <c r="N43" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="O43" s="14"/>
-      <c r="P43" s="15" t="s">
+      <c r="O43" s="22"/>
+      <c r="P43" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="Q43" s="13"/>
+      <c r="Q43" s="19"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M44" s="7" t="s">
@@ -8554,7 +8546,7 @@
         <f>N32/N32</f>
         <v>1</v>
       </c>
-      <c r="O45" s="19">
+      <c r="O45" s="13">
         <f>O32/O32</f>
         <v>1</v>
       </c>
@@ -8584,7 +8576,7 @@
         <f t="shared" ref="N46:N53" si="0">N33/N33</f>
         <v>1</v>
       </c>
-      <c r="O46" s="20">
+      <c r="O46" s="14">
         <f t="shared" ref="O46:O53" si="1">O33/O33</f>
         <v>1</v>
       </c>
@@ -8614,7 +8606,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O47" s="20">
+      <c r="O47" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8636,7 +8628,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O48" s="20">
+      <c r="O48" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8658,7 +8650,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O49" s="20">
+      <c r="O49" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8680,7 +8672,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O50" s="20">
+      <c r="O50" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8702,7 +8694,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O51" s="20">
+      <c r="O51" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8724,7 +8716,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O52" s="20">
+      <c r="O52" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8746,7 +8738,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O53" s="20">
+      <c r="O53" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8764,6 +8756,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="N15:Q15"/>
     <mergeCell ref="T15:W15"/>
     <mergeCell ref="B15:E15"/>
@@ -8780,23 +8789,6 @@
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>